<commit_message>
Add couple and guest gender fields, update views and routes, and modify app name.
</commit_message>
<xml_diff>
--- a/public/template_guests.xlsx
+++ b/public/template_guests.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8FA1FD-7B41-4C2A-ACA9-6470B6477B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778CD559-800D-42B1-9E00-ED07C3166E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6E2AB393-BDB7-486B-BBE6-46D40B55C5AE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>guest_name</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>guest_gender</t>
+  </si>
+  <si>
+    <t>Male</t>
   </si>
 </sst>
 </file>
@@ -422,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23225C8C-E757-4146-8A7E-9C544669A610}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,49 +445,55 @@
     <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add QR code auto generate for guest, update views, and modify app configuration
</commit_message>
<xml_diff>
--- a/public/template_guests.xlsx
+++ b/public/template_guests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778CD559-800D-42B1-9E00-ED07C3166E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43E0B54-EDDF-4C0C-BF6F-4CA11560BC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6E2AB393-BDB7-486B-BBE6-46D40B55C5AE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>guest_name</t>
   </si>
@@ -48,34 +48,109 @@
     <t>guest_address</t>
   </si>
   <si>
-    <t>guest_qr_code</t>
-  </si>
-  <si>
-    <t>guest_attendance_status</t>
-  </si>
-  <si>
-    <t>guest_invitation_status</t>
-  </si>
-  <si>
-    <t>Joko</t>
-  </si>
-  <si>
     <t>VIP</t>
   </si>
   <si>
     <t>081234567890</t>
   </si>
   <si>
-    <t>JALAN COBA-COBA</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>guest_gender</t>
   </si>
   <si>
     <t>Male</t>
+  </si>
+  <si>
+    <t>Nicholas Arthur</t>
+  </si>
+  <si>
+    <t>101st Fake Street</t>
+  </si>
+  <si>
+    <t>Emily Johnson</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Regular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">202nd Imaginary Avenue  </t>
+  </si>
+  <si>
+    <t>Michael Smith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">303rd Fantasy Lane  </t>
+  </si>
+  <si>
+    <t>Sophia Brown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">404th Fictional Road  </t>
+  </si>
+  <si>
+    <t>James Wilson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">505th Mythical Drive  </t>
+  </si>
+  <si>
+    <t>Olivia Martinez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">606th Dreamland Blvd  </t>
+  </si>
+  <si>
+    <t>Benjamin Taylor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">707th Illusion St  </t>
+  </si>
+  <si>
+    <t>Charlotte Anderson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">808th Fable Court  </t>
+  </si>
+  <si>
+    <t>William Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">909th Storybook Ave  </t>
+  </si>
+  <si>
+    <t>Ava Hernandez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1001st Legendary Way  </t>
+  </si>
+  <si>
+    <t>082198765432</t>
+  </si>
+  <si>
+    <t>081278945612</t>
+  </si>
+  <si>
+    <t>082345678901</t>
+  </si>
+  <si>
+    <t>081234569876</t>
+  </si>
+  <si>
+    <t>082156734589</t>
+  </si>
+  <si>
+    <t>081298734561</t>
+  </si>
+  <si>
+    <t>082312478956</t>
+  </si>
+  <si>
+    <t>081289734502</t>
+  </si>
+  <si>
+    <t>082376591234</t>
   </si>
 </sst>
 </file>
@@ -428,73 +503,207 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23225C8C-E757-4146-8A7E-9C544669A610}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.21875" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
         <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Update WhatsApp message format and enhance guest input fields in forms
</commit_message>
<xml_diff>
--- a/public/template_guests.xlsx
+++ b/public/template_guests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Laravel\SKRIPSI\skripsi-manajemen-tamu\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43E0B54-EDDF-4C0C-BF6F-4CA11560BC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADEF4DA-15C3-4ED2-9FA7-FD7A866C9F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6E2AB393-BDB7-486B-BBE6-46D40B55C5AE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6E2AB393-BDB7-486B-BBE6-46D40B55C5AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>guest_name</t>
   </si>
@@ -51,9 +51,6 @@
     <t>VIP</t>
   </si>
   <si>
-    <t>081234567890</t>
-  </si>
-  <si>
     <t>guest_gender</t>
   </si>
   <si>
@@ -78,79 +75,10 @@
     <t xml:space="preserve">202nd Imaginary Avenue  </t>
   </si>
   <si>
-    <t>Michael Smith</t>
-  </si>
-  <si>
-    <t xml:space="preserve">303rd Fantasy Lane  </t>
-  </si>
-  <si>
-    <t>Sophia Brown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">404th Fictional Road  </t>
-  </si>
-  <si>
-    <t>James Wilson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">505th Mythical Drive  </t>
-  </si>
-  <si>
-    <t>Olivia Martinez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">606th Dreamland Blvd  </t>
-  </si>
-  <si>
-    <t>Benjamin Taylor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">707th Illusion St  </t>
-  </si>
-  <si>
-    <t>Charlotte Anderson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">808th Fable Court  </t>
-  </si>
-  <si>
-    <t>William Thomas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">909th Storybook Ave  </t>
-  </si>
-  <si>
-    <t>Ava Hernandez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1001st Legendary Way  </t>
-  </si>
-  <si>
-    <t>082198765432</t>
-  </si>
-  <si>
-    <t>081278945612</t>
-  </si>
-  <si>
-    <t>082345678901</t>
-  </si>
-  <si>
-    <t>081234569876</t>
-  </si>
-  <si>
-    <t>082156734589</t>
-  </si>
-  <si>
-    <t>081298734561</t>
-  </si>
-  <si>
-    <t>082312478956</t>
-  </si>
-  <si>
-    <t>081289734502</t>
-  </si>
-  <si>
-    <t>082376591234</t>
+    <t>6281234567890</t>
+  </si>
+  <si>
+    <t>6282198765432</t>
   </si>
 </sst>
 </file>
@@ -503,9 +431,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23225C8C-E757-4146-8A7E-9C544669A610}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -524,7 +454,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -538,172 +468,36 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>